<commit_message>
- The optimization framework without the stress constraints is now working
</commit_message>
<xml_diff>
--- a/Enveloping Constraints.xlsx
+++ b/Enveloping Constraints.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,590 +411,1038 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-0.5099311615858596</v>
+        <v>-27.221717401181074</v>
       </c>
       <c r="B2">
-        <v>-0.5353716544423162</v>
+        <v>-2.1303952748750405</v>
       </c>
       <c r="C2">
-        <v>1.0</v>
+        <v>15.386188096319737</v>
       </c>
       <c r="D2">
-        <v>-0.22202576283503406</v>
+        <v>-13.492503407541925</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>-0.12897384508968632</v>
+        <v>-4.2205363037958135</v>
       </c>
       <c r="B3">
-        <v>-0.07530555569282676</v>
+        <v>-0.21116834893572603</v>
       </c>
       <c r="C3">
-        <v>0.1857383833868501</v>
+        <v>1.911109952260133</v>
       </c>
       <c r="D3">
-        <v>0.0014483947888980927</v>
+        <v>-2.7824725686651552</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-0.6011692717572288</v>
+        <v>-20.910815939278564</v>
       </c>
       <c r="B4">
-        <v>-11.113042800640606</v>
+        <v>-1.3244781783680946</v>
       </c>
       <c r="C4">
-        <v>12.1086123101198</v>
+        <v>10.755218216318582</v>
       </c>
       <c r="D4">
-        <v>-12.224161456995494</v>
+        <v>-9.137381404174374</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-0.7793647211291758</v>
+        <v>-14.465714786583728</v>
       </c>
       <c r="B5">
-        <v>-0.6251364286562391</v>
+        <v>-0.86981674089535</v>
       </c>
       <c r="C5">
-        <v>1.3459178092239337</v>
+        <v>7.257261069389131</v>
       </c>
       <c r="D5">
-        <v>-0.05958820908544809</v>
+        <v>-6.557877859237311</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>1.0869149441763946</v>
+        <v>0.8732875780794556</v>
       </c>
       <c r="B6">
-        <v>-7.961459264115453</v>
+        <v>-0.15377455179237887</v>
       </c>
       <c r="C6">
-        <v>7.340097570936264</v>
+        <v>0.3246351648952206</v>
       </c>
       <c r="D6">
-        <v>-9.963474663865806</v>
+        <v>0.9647929286524268</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>-4.706995830895032</v>
+        <v>-14.739538977844749</v>
       </c>
       <c r="B7">
-        <v>-10.325164424057991</v>
+        <v>-0.9123730112110109</v>
       </c>
       <c r="C7">
-        <v>15.133391064750342</v>
+        <v>7.522939312066166</v>
       </c>
       <c r="D7">
-        <v>-7.284433603863913</v>
+        <v>-6.029285881562995</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>0.5027973655679941</v>
+        <v>3.2880255725696657</v>
       </c>
       <c r="B8">
-        <v>-0.4024158187950821</v>
+        <v>0.08618585944083412</v>
       </c>
       <c r="C8">
-        <v>-0.028083680369972497</v>
+        <v>-1.236294111796011</v>
       </c>
       <c r="D8">
-        <v>-0.8722638900782945</v>
+        <v>1.9452253580500278</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>-3.2798842525021414</v>
+        <v>-1.493991685502053</v>
       </c>
       <c r="B9">
-        <v>-3.1231799464261254</v>
+        <v>-0.2218689144887091</v>
       </c>
       <c r="C9">
-        <v>6.29134930787339</v>
+        <v>1.254284064320646</v>
       </c>
       <c r="D9">
-        <v>-0.4553734227220572</v>
+        <v>0.047941524236167835</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>-0.1347662311741249</v>
+        <v>1.8037092375091426</v>
       </c>
       <c r="B10">
-        <v>-0.2363675739374443</v>
+        <v>0.01503091031259352</v>
       </c>
       <c r="C10">
-        <v>0.3838561817237274</v>
+        <v>-0.5511333781278573</v>
       </c>
       <c r="D10">
-        <v>-0.09535743814943136</v>
+        <v>1.3628025350068986</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>-0.25625898375632244</v>
+        <v>2.09759755164783</v>
       </c>
       <c r="B11">
-        <v>-0.27502301804655677</v>
+        <v>0.032243475878348075</v>
       </c>
       <c r="C11">
-        <v>0.535866074207935</v>
+        <v>-0.698018104180016</v>
       </c>
       <c r="D11">
-        <v>-0.026838970724480517</v>
+        <v>1.478948003476303</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>0.23703923446065212</v>
+        <v>-11.136117104189506</v>
       </c>
       <c r="B12">
-        <v>0.04604431454133811</v>
+        <v>-0.6969571078103763</v>
       </c>
       <c r="C12">
-        <v>-0.26224604589281186</v>
+        <v>5.722529697350441</v>
       </c>
       <c r="D12">
-        <v>-0.14988657485395027</v>
+        <v>-4.291625904784617</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>-0.08939090851419461</v>
+        <v>1.8036856781262693</v>
       </c>
       <c r="B13">
-        <v>-0.23805723085047728</v>
+        <v>0.021719775181622887</v>
       </c>
       <c r="C13">
-        <v>0.34394740432276943</v>
+        <v>-0.5760462113387468</v>
       </c>
       <c r="D13">
-        <v>-0.13919201079938212</v>
+        <v>1.347570399312174</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>-0.17172285793008282</v>
+        <v>-0.09388440754154193</v>
       </c>
       <c r="B14">
-        <v>-0.19972417533461398</v>
+        <v>-0.028165322262483257</v>
       </c>
       <c r="C14">
-        <v>0.3783751982990112</v>
+        <v>0.14082661131239785</v>
       </c>
       <c r="D14">
-        <v>-0.023389165359078624</v>
+        <v>0.3943145116748371</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>0.17099384067636803</v>
+        <v>-1.2850132824832872</v>
       </c>
       <c r="B15">
-        <v>0.12531607817415877</v>
+        <v>-0.08398333355230807</v>
       </c>
       <c r="C15">
-        <v>-0.2868897898885978</v>
+        <v>0.6821085383638684</v>
       </c>
       <c r="D15">
-        <v>-0.007094899338830799</v>
+        <v>-0.14830227680947985</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>-1.2540561337570912</v>
+        <v>3.169814486274228</v>
       </c>
       <c r="B16">
-        <v>-1.0824117462311924</v>
+        <v>0.0931630819619184</v>
       </c>
       <c r="C16">
-        <v>2.267084513195921</v>
+        <v>-1.2310674530913575</v>
       </c>
       <c r="D16">
-        <v>-0.11535100760348553</v>
+        <v>1.8271767077435337</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>-0.285185588149065</v>
+        <v>-0.2050265227454402</v>
       </c>
       <c r="B17">
-        <v>-0.2979796683882363</v>
+        <v>-0.026280672461012664</v>
       </c>
       <c r="C17">
-        <v>0.5864404985594185</v>
+        <v>0.16402121819637827</v>
       </c>
       <c r="D17">
-        <v>-0.026083990298614503</v>
+        <v>0.31052198808550047</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>-0.12826391652556304</v>
+        <v>-0.512432192087778</v>
       </c>
       <c r="B18">
-        <v>-0.154278946062536</v>
+        <v>-0.03452433852737582</v>
       </c>
       <c r="C18">
-        <v>0.28946118835681445</v>
+        <v>0.27998872351187815</v>
       </c>
       <c r="D18">
-        <v>-0.01697535212524238</v>
+        <v>0.14167525460721436</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>-0.26126966535069335</v>
+        <v>0.3839823189155516</v>
       </c>
       <c r="B19">
-        <v>-0.27024116784440044</v>
+        <v>0.010454040932394704</v>
       </c>
       <c r="C19">
-        <v>0.5342882976703979</v>
+        <v>-0.1415856145830875</v>
       </c>
       <c r="D19">
-        <v>-0.020673830404329685</v>
+        <v>0.4827992339732909</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>-0.4564066331300123</v>
+        <v>-1.6047215004057904</v>
       </c>
       <c r="B20">
-        <v>-0.3490454162062884</v>
+        <v>-0.06354831992153218</v>
       </c>
       <c r="C20">
-        <v>0.7668256284244092</v>
+        <v>0.6472344611030454</v>
       </c>
       <c r="D20">
-        <v>-0.02510811764466399</v>
+        <v>-1.3001711738761905</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>-0.28405743961093316</v>
+        <v>-1.2545459091646785</v>
       </c>
       <c r="B21">
-        <v>-0.2623793935097797</v>
+        <v>-0.0456405165665505</v>
       </c>
       <c r="C21">
-        <v>0.5403070931165787</v>
+        <v>0.4850894010357768</v>
       </c>
       <c r="D21">
-        <v>-0.012699459317038449</v>
+        <v>-1.0948015754199085</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>0.06292918225568311</v>
+        <v>-0.34357750305210644</v>
       </c>
       <c r="B22">
-        <v>0.0737739624985162</v>
+        <v>-0.0228258097768772</v>
       </c>
       <c r="C22">
-        <v>-0.13823974396791677</v>
+        <v>0.1877279140387793</v>
       </c>
       <c r="D22">
-        <v>0.019649190019267068</v>
+        <v>0.1826297046813393</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>-0.31043167185104453</v>
+        <v>-1.1864855487073929</v>
       </c>
       <c r="B23">
-        <v>-0.23750338431830514</v>
+        <v>-0.04501175789993911</v>
       </c>
       <c r="C23">
-        <v>0.5230997752746972</v>
+        <v>0.47008651078180236</v>
       </c>
       <c r="D23">
-        <v>-0.01083182851453803</v>
+        <v>-0.9353647989490307</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>-0.2327315221591199</v>
+        <v>-0.22568965211608705</v>
       </c>
       <c r="B24">
-        <v>-0.18057383069991542</v>
+        <v>-0.015324380008328312</v>
       </c>
       <c r="C24">
-        <v>0.3966903569830741</v>
+        <v>0.12596791391047876</v>
       </c>
       <c r="D24">
-        <v>-0.0034740052375662367</v>
+        <v>0.21603325617234917</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>-0.009355079958181196</v>
+        <v>-0.3338727484604786</v>
       </c>
       <c r="B25">
-        <v>0.003493798870721675</v>
+        <v>-0.015827743081419827</v>
       </c>
       <c r="C25">
-        <v>0.004429402509677274</v>
+        <v>0.15129657720746395</v>
       </c>
       <c r="D25">
-        <v>0.016073395072000275</v>
+        <v>0.025399567353739473</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>-0.16374819294732118</v>
+        <v>-0.02819200531688978</v>
       </c>
       <c r="B26">
-        <v>-0.1395233187785208</v>
+        <v>-0.0037304788261860265</v>
       </c>
       <c r="C26">
-        <v>0.2973725693644685</v>
+        <v>0.026377985292711903</v>
       </c>
       <c r="D26">
-        <v>0.0021209204609783185</v>
+        <v>0.27902402355377925</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>-0.018540400684144292</v>
+        <v>-0.3522005921677528</v>
       </c>
       <c r="B27">
-        <v>-0.005740263660592147</v>
+        <v>-0.014533519278626153</v>
       </c>
       <c r="C27">
-        <v>0.022913971568739835</v>
+        <v>0.14869330589220253</v>
       </c>
       <c r="D27">
-        <v>0.015400603472911669</v>
+        <v>-0.04373009511291802</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>-0.25154034896102706</v>
+        <v>0.05445458316721138</v>
       </c>
       <c r="B28">
-        <v>-0.2512585766593521</v>
+        <v>0.0008288503995012141</v>
       </c>
       <c r="C28">
-        <v>0.5032678259349774</v>
+        <v>-0.014132770808657024</v>
       </c>
       <c r="D28">
-        <v>-0.015525491027337265</v>
+        <v>0.30749536337154015</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>-0.022305587454493826</v>
+        <v>-0.07960138012685679</v>
       </c>
       <c r="B29">
-        <v>-0.00964014688744543</v>
+        <v>-0.003633652839559935</v>
       </c>
       <c r="C29">
-        <v>0.03062548659681441</v>
+        <v>0.03673498132563284</v>
       </c>
       <c r="D29">
-        <v>0.015042597926189349</v>
+        <v>0.17946141556952225</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>-0.2081001790264968</v>
+        <v>-0.5883135529952503</v>
       </c>
       <c r="B30">
-        <v>-0.21815527868353346</v>
+        <v>-0.014665405100683945</v>
       </c>
       <c r="C30">
-        <v>0.4296547061737255</v>
+        <v>0.1883669831767372</v>
       </c>
       <c r="D30">
-        <v>-0.015247771669309525</v>
+        <v>-0.6924904772740407</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>-0.05648784188897563</v>
+        <v>-0.3206993717940573</v>
       </c>
       <c r="B31">
-        <v>-0.047786889022019274</v>
+        <v>-0.013133805784177959</v>
       </c>
       <c r="C31">
-        <v>0.10384809448918202</v>
+        <v>0.1350551726863588</v>
       </c>
       <c r="D31">
-        <v>0.00982929593136524</v>
+        <v>-0.021680147882102374</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>-0.17567552536040226</v>
+        <v>-0.19409898737701597</v>
       </c>
       <c r="B32">
-        <v>-0.18901584342246922</v>
+        <v>-0.007763959495080645</v>
       </c>
       <c r="C32">
-        <v>0.3689432077085201</v>
+        <v>0.08152157469834673</v>
       </c>
       <c r="D32">
-        <v>-0.013746924834993209</v>
+        <v>0.07375761520326278</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>-0.09425714824606439</v>
+        <v>-0.21859043142680504</v>
       </c>
       <c r="B33">
-        <v>-0.0911957659888455</v>
+        <v>-0.0065418626148827244</v>
       </c>
       <c r="C33">
-        <v>0.18622723335527644</v>
+        <v>0.07844111147525906</v>
       </c>
       <c r="D33">
-        <v>0.0031569609819255147</v>
+        <v>-0.04611004486259733</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>-0.10672374907890075</v>
+        <v>-0.05911900682344844</v>
       </c>
       <c r="B34">
-        <v>-0.1332989084519992</v>
+        <v>-0.0028432742130012453</v>
       </c>
       <c r="C34">
-        <v>0.24705515145814477</v>
+        <v>0.028413563214578927</v>
       </c>
       <c r="D34">
-        <v>-0.015384772249141473</v>
+        <v>0.1959941315427541</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>-0.06367344639462401</v>
+        <v>-0.21744210089598298</v>
       </c>
       <c r="B35">
-        <v>-0.056106281969240036</v>
+        <v>-0.0065143476855448875</v>
       </c>
       <c r="C35">
-        <v>0.11959717163217741</v>
+        <v>0.07808148168537586</v>
       </c>
       <c r="D35">
-        <v>0.00853312730566698</v>
+        <v>-0.04429387515494999</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>-0.030328523228972882</v>
+        <v>-0.02957863581920605</v>
       </c>
       <c r="B36">
-        <v>-0.01888932991850763</v>
+        <v>-0.0017486576770650477</v>
       </c>
       <c r="C36">
-        <v>0.0481948739241302</v>
+        <v>0.01664134879261533</v>
       </c>
       <c r="D36">
-        <v>0.013727496498213877</v>
+        <v>0.22110225728399777</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>-0.03107441725022242</v>
+        <v>-0.14202295962053385</v>
       </c>
       <c r="B37">
-        <v>-0.05996281327241676</v>
+        <v>-0.004196132897879438</v>
       </c>
       <c r="C37">
-        <v>0.09849735499795108</v>
+        <v>0.050999153681919145</v>
       </c>
       <c r="D37">
-        <v>-0.010154495535834945</v>
+        <v>0.043898005700892445</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>-0.027819709479598116</v>
+        <v>0.008199588318623602</v>
       </c>
       <c r="B38">
-        <v>-0.029063277990503584</v>
+        <v>-0.000494133085517088</v>
       </c>
       <c r="C38">
-        <v>0.05852575129711547</v>
+        <v>0.0023217781660104958</v>
       </c>
       <c r="D38">
-        <v>0.00645598434379552</v>
+        <v>0.2572685568560218</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>-0.02815599689021019</v>
+        <v>-0.08802790946011944</v>
       </c>
       <c r="B39">
-        <v>-0.03933671899118567</v>
+        <v>-0.002636462622372662</v>
       </c>
       <c r="C39">
-        <v>0.07122592688808078</v>
+        <v>0.032163482987167945</v>
       </c>
       <c r="D39">
-        <v>0.0005579066936565942</v>
+        <v>0.11073726302156542</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>-0.013836768749107223</v>
+        <v>0.02235162129409251</v>
       </c>
       <c r="B40">
-        <v>-0.0010393444590583861</v>
+        <v>-5.425793209331066e-5</v>
       </c>
       <c r="C40">
-        <v>0.013487498995691296</v>
+        <v>-0.002890227407123202</v>
       </c>
       <c r="D40">
-        <v>0.015747304676876378</v>
+        <v>0.2716562323497202</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>-0.02616026141050189</v>
+        <v>-0.014496300500744908</v>
       </c>
       <c r="B41">
-        <v>-0.02973167532449669</v>
+        <v>-0.0008792321390668622</v>
       </c>
       <c r="C41">
-        <v>0.058018247987474174</v>
+        <v>0.008603239210224264</v>
       </c>
       <c r="D41">
-        <v>0.005210123377738013</v>
+        <v>0.21649909660892233</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>0.07701500300494621</v>
+        <v>0.039537993069698386</v>
       </c>
       <c r="B42">
-        <v>0.08056141822637909</v>
+        <v>0.00047009344962388856</v>
       </c>
       <c r="C42">
-        <v>-0.15768779870956867</v>
+        <v>-0.009169956223996443</v>
       </c>
       <c r="D42">
-        <v>0.016242116612998823</v>
+        <v>0.2894033169963023</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>-0.0034654767545751236</v>
+        <v>-0.05823485627468608</v>
       </c>
       <c r="B43">
-        <v>-0.034556479014944214</v>
+        <v>-0.0017043697630316657</v>
       </c>
       <c r="C43">
-        <v>0.045742838360119525</v>
+        <v>0.021231272791442896</v>
       </c>
       <c r="D43">
-        <v>-0.009642514651528168</v>
+        <v>0.14221752075875926</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>-0.01161258542885767</v>
+      </c>
+      <c r="B44">
+        <v>-0.0005999835804910793</v>
+      </c>
+      <c r="C44">
+        <v>0.006290150440632013</v>
+      </c>
+      <c r="D44">
+        <v>0.20854267999329784</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>-0.050525518984240576</v>
+      </c>
+      <c r="B45">
+        <v>-0.0014801004973030633</v>
+      </c>
+      <c r="C45">
+        <v>0.018486395769528135</v>
+      </c>
+      <c r="D45">
+        <v>0.15080381372119997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>0.043728678221739266</v>
+      </c>
+      <c r="B46">
+        <v>0.0005922620989197584</v>
+      </c>
+      <c r="C46">
+        <v>-0.010672406187329968</v>
+      </c>
+      <c r="D46">
+        <v>0.29388946678426214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>-0.03880874505183148</v>
+      </c>
+      <c r="B47">
+        <v>-0.0011130149061659882</v>
+      </c>
+      <c r="C47">
+        <v>0.014127875842907152</v>
+      </c>
+      <c r="D47">
+        <v>0.16208372861296222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>-0.44417449426658373</v>
+      </c>
+      <c r="B48">
+        <v>-0.008836237279558784</v>
+      </c>
+      <c r="C48">
+        <v>0.12748753037566515</v>
+      </c>
+      <c r="D48">
+        <v>-0.6021872079716253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>-0.345237629892223</v>
+      </c>
+      <c r="B49">
+        <v>-0.004863930492669692</v>
+      </c>
+      <c r="C49">
+        <v>0.08580954684418919</v>
+      </c>
+      <c r="D49">
+        <v>-0.5400953122720982</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>-0.30771258178770106</v>
+      </c>
+      <c r="B50">
+        <v>-0.008212109718039172</v>
+      </c>
+      <c r="C50">
+        <v>0.10320030929086632</v>
+      </c>
+      <c r="D50">
+        <v>-0.21535928372867713</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>-0.2924412246644996</v>
+      </c>
+      <c r="B51">
+        <v>-0.004420425786381755</v>
+      </c>
+      <c r="C51">
+        <v>0.0751231912522118</v>
+      </c>
+      <c r="D51">
+        <v>-0.40120491705326283</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>-0.1283506034199154</v>
+      </c>
+      <c r="B52">
+        <v>-0.0037559612839344883</v>
+      </c>
+      <c r="C52">
+        <v>0.04595461387020549</v>
+      </c>
+      <c r="D52">
+        <v>0.05867456156339771</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>-0.269433808391932</v>
+      </c>
+      <c r="B53">
+        <v>-0.004208899224820297</v>
+      </c>
+      <c r="C53">
+        <v>0.07030409739168958</v>
+      </c>
+      <c r="D53">
+        <v>-0.342530208114593</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>-0.06566475370639195</v>
+      </c>
+      <c r="B54">
+        <v>-0.0019018698411294376</v>
+      </c>
+      <c r="C54">
+        <v>0.023737484308812885</v>
+      </c>
+      <c r="D54">
+        <v>0.1325613003948619</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>-0.16184091420717683</v>
+      </c>
+      <c r="B55">
+        <v>-0.0029979102679330094</v>
+      </c>
+      <c r="C55">
+        <v>0.04587033911243462</v>
+      </c>
+      <c r="D55">
+        <v>-0.0892128772791434</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>-0.06316493813167455</v>
+      </c>
+      <c r="B56">
+        <v>-0.0018302110184858747</v>
+      </c>
+      <c r="C56">
+        <v>0.02286145344970725</v>
+      </c>
+      <c r="D56">
+        <v>0.13554104440085996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>-0.07073294845827037</v>
+      </c>
+      <c r="B57">
+        <v>-0.001938082787756481</v>
+      </c>
+      <c r="C57">
+        <v>0.024756531960393676</v>
+      </c>
+      <c r="D57">
+        <v>0.11953868289444354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>-0.03470915373391988</v>
+      </c>
+      <c r="B58">
+        <v>-0.0009641431592755642</v>
+      </c>
+      <c r="C58">
+        <v>0.012457394544156977</v>
+      </c>
+      <c r="D58">
+        <v>0.16465237918318543</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>-0.17549781943683812</v>
+      </c>
+      <c r="B59">
+        <v>-0.003073869108608552</v>
+      </c>
+      <c r="C59">
+        <v>0.04844495661708684</v>
+      </c>
+      <c r="D59">
+        <v>-0.12609624617275178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>-0.023843065885896915</v>
+      </c>
+      <c r="B60">
+        <v>-0.0006623073857193684</v>
+      </c>
+      <c r="C60">
+        <v>0.008663777365974068</v>
+      </c>
+      <c r="D60">
+        <v>0.17721054954651763</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>-0.09489842045785957</v>
+      </c>
+      <c r="B61">
+        <v>-0.0018170011244503838</v>
+      </c>
+      <c r="C61">
+        <v>0.027493155939422757</v>
+      </c>
+      <c r="D61">
+        <v>0.03704253275339297</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>-0.22868506047316745</v>
+      </c>
+      <c r="B62">
+        <v>-0.0037010293986935176</v>
+      </c>
+      <c r="C62">
+        <v>0.06071673294091851</v>
+      </c>
+      <c r="D62">
+        <v>-0.24958566486496586</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>-0.00941027584567987</v>
+      </c>
+      <c r="B63">
+        <v>-0.00033716169397530256</v>
+      </c>
+      <c r="C63">
+        <v>0.004142853016050792</v>
+      </c>
+      <c r="D63">
+        <v>0.1985876100011551</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>-0.3027057446247986</v>
+      </c>
+      <c r="B64">
+        <v>-0.004498636341605904</v>
+      </c>
+      <c r="C64">
+        <v>0.07714555773947067</v>
+      </c>
+      <c r="D64">
+        <v>-0.4287131979856655</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>0.0014083007529090863</v>
+      </c>
+      <c r="B65">
+        <v>-0.00010899861991699303</v>
+      </c>
+      <c r="C65">
+        <v>0.0008604138846545667</v>
+      </c>
+      <c r="D65">
+        <v>0.21557612004641608</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>-0.3087107361832951</v>
+      </c>
+      <c r="B66">
+        <v>-0.003714111690884662</v>
+      </c>
+      <c r="C66">
+        <v>0.07162646282460491</v>
+      </c>
+      <c r="D66">
+        <v>-0.5159863737023885</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>0.004311181415417839</v>
+      </c>
+      <c r="B67">
+        <v>-5.039689181893807e-5</v>
+      </c>
+      <c r="C67">
+        <v>-2.4336884665030444e-6</v>
+      </c>
+      <c r="D67">
+        <v>0.22029694705462993</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>-0.3035608127432514</v>
+      </c>
+      <c r="B68">
+        <v>-0.0035562405286433487</v>
+      </c>
+      <c r="C68">
+        <v>0.06964291741691774</v>
+      </c>
+      <c r="D68">
+        <v>-0.5125713873154985</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>0.0036208595363976413</v>
+      </c>
+      <c r="B69">
+        <v>-5.679779664935831e-5</v>
+      </c>
+      <c r="C69">
+        <v>0.00014199449162327217</v>
+      </c>
+      <c r="D69">
+        <v>0.21852952260842984</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>-0.07233102414388348</v>
+      </c>
+      <c r="B70">
+        <v>-0.0009041378017985342</v>
+      </c>
+      <c r="C70">
+        <v>0.01717861823417224</v>
+      </c>
+      <c r="D70">
+        <v>0.03616551207192713</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>2.9591992396461435e-17</v>
+      </c>
+      <c r="B71">
+        <v>-8.705502518425259e-5</v>
+      </c>
+      <c r="C71">
+        <v>0.0008705502518425227</v>
+      </c>
+      <c r="D71">
+        <v>0.20893206044220766</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>-0.2622300086536612</v>
+      </c>
+      <c r="B72">
+        <v>-0.0023582159809798333</v>
+      </c>
+      <c r="C72">
+        <v>0.05398616511128953</v>
+      </c>
+      <c r="D72">
+        <v>-0.4849063038081583</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>-0.004461016777400653</v>
+      </c>
+      <c r="B73">
+        <v>-0.00011598643621240854</v>
+      </c>
+      <c r="C73">
+        <v>0.0016951863754121653</v>
+      </c>
+      <c r="D73">
+        <v>0.1962847382056106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>0.04391570439904369</v>
+      </c>
+      <c r="B74">
+        <v>0.0005964699832991099</v>
+      </c>
+      <c r="C74">
+        <v>-0.010733161734199375</v>
+      </c>
+      <c r="D74">
+        <v>0.29412440784339056</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>-0.004538964134787244</v>
+      </c>
+      <c r="B75">
+        <v>-0.00011515520119737932</v>
+      </c>
+      <c r="C75">
+        <v>0.0016979088059759584</v>
+      </c>
+      <c r="D75">
+        <v>0.19593195181830797</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +1452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1026,1010 +1474,2018 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-0.48512680228818117</v>
+        <v>-0.8148841563304399</v>
       </c>
       <c r="B2">
-        <v>-0.5123455393200839</v>
+        <v>-0.26068336063655584</v>
       </c>
       <c r="C2">
         <v>1.0</v>
       </c>
       <c r="D2">
-        <v>-0.05642658765099351</v>
+        <v>0.2132717060613345</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>-18.796747371625646</v>
+        <v>-31.60991365567991</v>
       </c>
       <c r="B3">
-        <v>-15.590525666075045</v>
+        <v>-5.440479244730908</v>
       </c>
       <c r="C3">
-        <v>32.38151675545328</v>
+        <v>24.70613862351656</v>
       </c>
       <c r="D3">
-        <v>-3.548612781454574</v>
+        <v>-27.388834211029337</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-0.3048458201937994</v>
+        <v>0.5770811366628023</v>
       </c>
       <c r="B4">
-        <v>-0.3573299506047028</v>
+        <v>0.00928716839204997</v>
       </c>
       <c r="C4">
-        <v>0.677090419842527</v>
+        <v>-0.21384546847883423</v>
       </c>
       <c r="D4">
-        <v>-0.03175574905635494</v>
+        <v>0.972216214201619</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-0.5492784804905345</v>
+        <v>-2.5743298416586633</v>
       </c>
       <c r="B5">
-        <v>-0.5608658090959878</v>
+        <v>-0.4160603941630424</v>
       </c>
       <c r="C5">
-        <v>1.1109339301973196</v>
+        <v>2.145622485689734</v>
       </c>
       <c r="D5">
-        <v>-0.05322582392965887</v>
+        <v>-0.36644145210927054</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>3.471735243422574</v>
+        <v>-0.4547719864488147</v>
       </c>
       <c r="B6">
-        <v>3.1797749614614044</v>
+        <v>0.006368727717774154</v>
       </c>
       <c r="C6">
-        <v>-6.702924781899716</v>
+        <v>-0.09708832453348021</v>
       </c>
       <c r="D6">
-        <v>0.056645282439001444</v>
+        <v>-2.279524762958368</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>-19.073099661947953</v>
+        <v>-3.8845950154015947</v>
       </c>
       <c r="B7">
-        <v>-15.621343326881668</v>
+        <v>-0.5861584422856954</v>
       </c>
       <c r="C7">
-        <v>32.90055867446345</v>
+        <v>3.079563389673578</v>
       </c>
       <c r="D7">
-        <v>-2.8957097906177443</v>
+        <v>-1.1840377448988302</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>3.3346501303029497</v>
+        <v>-1.270914948947481</v>
       </c>
       <c r="B8">
-        <v>2.9210123995130837</v>
+        <v>-0.22063816733891134</v>
       </c>
       <c r="C8">
-        <v>-6.158092664892056</v>
+        <v>1.1289757457549332</v>
       </c>
       <c r="D8">
-        <v>0.246168519654144</v>
+        <v>0.22704773359586167</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>-4.499406474260262</v>
+        <v>-1.1524908891708292</v>
       </c>
       <c r="B9">
-        <v>-3.3746095030754324</v>
+        <v>-0.11127706818288625</v>
       </c>
       <c r="C9">
-        <v>7.3152782694895935</v>
+        <v>0.7305191331524281</v>
       </c>
       <c r="D9">
-        <v>-0.6658798847883879</v>
+        <v>-0.48725705823307425</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>-3.817283791433869</v>
+        <v>0.3468218493533306</v>
       </c>
       <c r="B10">
-        <v>-3.2006100436757827</v>
+        <v>0.0015121206146776517</v>
       </c>
       <c r="C10">
-        <v>6.723300726202804</v>
+        <v>-0.09018100828858794</v>
       </c>
       <c r="D10">
-        <v>-0.4928272489918467</v>
+        <v>0.9219985584229199</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>-0.45332831209710567</v>
+        <v>-0.7343970127858094</v>
       </c>
       <c r="B11">
-        <v>-0.2664491469658435</v>
+        <v>-0.08156350769928085</v>
       </c>
       <c r="C11">
-        <v>0.6548151626532165</v>
+        <v>0.5145814252966283</v>
       </c>
       <c r="D11">
-        <v>0.003405327834074513</v>
+        <v>-0.02037644688316662</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>-1.3566324895273763</v>
+        <v>-1.1078070317667554</v>
       </c>
       <c r="B12">
-        <v>-1.208133823663559</v>
+        <v>-0.10357076986618882</v>
       </c>
       <c r="C12">
-        <v>2.4985837835209614</v>
+        <v>0.6883072618937629</v>
       </c>
       <c r="D12">
-        <v>-0.14434265308703192</v>
+        <v>-0.5086787030965196</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>-1.1124050185963414</v>
+        <v>-0.5085731523328113</v>
       </c>
       <c r="B13">
-        <v>-0.8922714637853654</v>
+        <v>-0.0012979694396761882</v>
       </c>
       <c r="C13">
-        <v>1.9210591460050885</v>
+        <v>0.054903444958338855</v>
       </c>
       <c r="D13">
-        <v>-0.08505160810946737</v>
+        <v>-1.378421222244109</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>-0.4856328749354555</v>
+        <v>-0.6868605548041382</v>
       </c>
       <c r="B14">
-        <v>-0.5063798520351566</v>
+        <v>-0.05375430428901928</v>
       </c>
       <c r="C14">
-        <v>0.9970789043652756</v>
+        <v>0.3882255309762511</v>
       </c>
       <c r="D14">
-        <v>-0.044949199372402694</v>
+        <v>-0.3404439271637901</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>-0.47706641859406856</v>
+        <v>-0.4209772407298933</v>
       </c>
       <c r="B15">
-        <v>-0.4990979500734398</v>
+        <v>-0.02106297931485585</v>
       </c>
       <c r="C15">
-        <v>0.9817853667738953</v>
+        <v>0.19062359295673825</v>
       </c>
       <c r="D15">
-        <v>-0.04392846121104162</v>
+        <v>-0.27753762556426465</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>-1.1629332211905863</v>
+        <v>-0.44533065828374274</v>
       </c>
       <c r="B16">
-        <v>-1.0037609520141226</v>
+        <v>-0.02820696910000472</v>
       </c>
       <c r="C16">
-        <v>2.102352378552222</v>
+        <v>0.22905028776336225</v>
       </c>
       <c r="D16">
-        <v>-0.10696930960977594</v>
+        <v>-0.1945957578856211</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>-0.47687676802826867</v>
+        <v>-0.42467181124026543</v>
       </c>
       <c r="B17">
-        <v>-0.4982705546987283</v>
+        <v>-0.02553531963354624</v>
       </c>
       <c r="C17">
-        <v>0.9806240610157534</v>
+        <v>0.21305232741345834</v>
       </c>
       <c r="D17">
-        <v>-0.043616681584846606</v>
+        <v>-0.1925204464115167</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>-0.35842827446827485</v>
+        <v>-0.8412707483469494</v>
       </c>
       <c r="B18">
-        <v>-0.4008838926231207</v>
+        <v>-0.08714411379155568</v>
       </c>
       <c r="C18">
-        <v>0.7715579891370412</v>
+        <v>0.5630475006208611</v>
       </c>
       <c r="D18">
-        <v>-0.034543828301001306</v>
+        <v>-0.15661784451616695</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>-0.4368222797193713</v>
+        <v>-0.4201554007172597</v>
       </c>
       <c r="B19">
-        <v>-0.4518219244984494</v>
+        <v>-0.02600749241242738</v>
       </c>
       <c r="C19">
-        <v>0.8932879058213467</v>
+        <v>0.21444385648586717</v>
       </c>
       <c r="D19">
-        <v>-0.034565014333484044</v>
+        <v>-0.17186677476241163</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>-0.8330853592390067</v>
+        <v>-0.21320253136667144</v>
       </c>
       <c r="B20">
-        <v>-0.6371174405524235</v>
+        <v>-0.03711467489903599</v>
       </c>
       <c r="C20">
-        <v>1.3996974578317447</v>
+        <v>0.20891779580906308</v>
       </c>
       <c r="D20">
-        <v>-0.04583019546488251</v>
+        <v>0.4017161209513987</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>-0.4390842788907491</v>
+        <v>-0.41442836075691786</v>
       </c>
       <c r="B21">
-        <v>-0.4055752489807389</v>
+        <v>-0.025937118746629524</v>
       </c>
       <c r="C21">
-        <v>0.8351844284930352</v>
+        <v>0.21296279301548543</v>
       </c>
       <c r="D21">
-        <v>-0.019630300632723655</v>
+        <v>-0.15971199584752535</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>-0.5297517866938576</v>
+        <v>-0.16668265457517042</v>
       </c>
       <c r="B22">
-        <v>-0.34258916800834843</v>
+        <v>-0.03348369496879374</v>
       </c>
       <c r="C22">
-        <v>0.8070620070866015</v>
+        <v>0.18271579095855864</v>
       </c>
       <c r="D22">
-        <v>-0.006237055569804471</v>
+        <v>0.4418484532014179</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>-0.5990078759297622</v>
+        <v>-0.31619876541516795</v>
       </c>
       <c r="B23">
-        <v>-0.45828570557356263</v>
+        <v>-0.020665487856570693</v>
       </c>
       <c r="C23">
-        <v>1.0093715097375109</v>
+        <v>0.16784408429848846</v>
       </c>
       <c r="D23">
-        <v>-0.020901058684668242</v>
+        <v>-0.03649222733694511</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>-0.5629534455641237</v>
+        <v>0.004515690090245515</v>
       </c>
       <c r="B24">
-        <v>-0.4319510335131833</v>
+        <v>-0.021512451479069144</v>
       </c>
       <c r="C24">
-        <v>0.9508619068459369</v>
+        <v>0.09075796804314608</v>
       </c>
       <c r="D24">
-        <v>-0.01733588950132881</v>
+        <v>0.5997058522955676</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>-0.5763117183383633</v>
+        <v>-0.17662333125080928</v>
       </c>
       <c r="B25">
-        <v>-0.43977786065495467</v>
+        <v>-0.022639899733056742</v>
       </c>
       <c r="C25">
-        <v>0.9699098737973942</v>
+        <v>0.14129866500064092</v>
       </c>
       <c r="D25">
-        <v>-0.01834830952240469</v>
+        <v>0.26750406351255007</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>-0.41295221345484845</v>
+        <v>0.37514120938421763</v>
       </c>
       <c r="B26">
-        <v>-0.41248962963421104</v>
+        <v>0.004530222941548219</v>
       </c>
       <c r="C26">
-        <v>0.8262116337950149</v>
+        <v>-0.10970209363130318</v>
       </c>
       <c r="D26">
-        <v>-0.025488101257687377</v>
+        <v>0.9323857014158513</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>-0.36094478317233974</v>
+        <v>-0.22730079654626792</v>
       </c>
       <c r="B27">
-        <v>-0.32015064919522934</v>
+        <v>-0.015314044996925857</v>
       </c>
       <c r="C27">
-        <v>0.6706345718758576</v>
+        <v>0.12419528058713622</v>
       </c>
       <c r="D27">
-        <v>-0.005471520891036632</v>
+        <v>0.0628432380329349</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>-0.3859490484081686</v>
+        <v>-0.3823165352923346</v>
       </c>
       <c r="B28">
-        <v>-0.40459754819532934</v>
+        <v>-0.015140056071975853</v>
       </c>
       <c r="C28">
-        <v>0.7968509482672195</v>
+        <v>0.15420023762886212</v>
       </c>
       <c r="D28">
-        <v>-0.02827899040570119</v>
+        <v>-0.30975900700377945</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>-0.24043160029880956</v>
+        <v>-0.37420517786292157</v>
       </c>
       <c r="B29">
-        <v>-0.227489706052596</v>
+        <v>-0.01361362505331796</v>
       </c>
       <c r="C29">
-        <v>0.4675890806780823</v>
+        <v>0.1446921665185425</v>
       </c>
       <c r="D29">
-        <v>0.004696155936023306</v>
+        <v>-0.32655673679362446</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>-0.36068129896563583</v>
+        <v>-0.1861639787031472</v>
       </c>
       <c r="B30">
-        <v>-0.388070448577506</v>
+        <v>-0.012367933078960185</v>
       </c>
       <c r="C30">
-        <v>0.7574812434905664</v>
+        <v>0.10171846259037949</v>
       </c>
       <c r="D30">
-        <v>-0.02822395832371021</v>
+        <v>0.09895604965643041</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>-0.21010286696555566</v>
+        <v>-0.35505156905706353</v>
       </c>
       <c r="B31">
-        <v>-0.20327892627685074</v>
+        <v>-0.013469608024978475</v>
       </c>
       <c r="C31">
-        <v>0.4151077808217333</v>
+        <v>0.1406717118699613</v>
       </c>
       <c r="D31">
-        <v>0.007036989401246353</v>
+        <v>-0.2799045802701993</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>-0.27881398726032636</v>
+        <v>-0.1463337795391864</v>
       </c>
       <c r="B32">
-        <v>-0.33407565561078023</v>
+        <v>-0.009936097754982672</v>
       </c>
       <c r="C32">
-        <v>0.6286140048355985</v>
+        <v>0.0816757027641921</v>
       </c>
       <c r="D32">
-        <v>-0.02948054865651022</v>
+        <v>0.14007271749260475</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>-0.20675863406698336</v>
+        <v>-0.19333737013791097</v>
       </c>
       <c r="B33">
-        <v>-0.19933456186753923</v>
+        <v>-0.009165450719444471</v>
       </c>
       <c r="C33">
-        <v>0.4077007659141519</v>
+        <v>0.08761206921810176</v>
       </c>
       <c r="D33">
-        <v>0.007749905644371588</v>
+        <v>0.014708255098530887</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>-0.11475953373138503</v>
+        <v>-0.027963142265786056</v>
       </c>
       <c r="B34">
-        <v>-0.18739254401083172</v>
+        <v>-0.003700194752505085</v>
       </c>
       <c r="C34">
-        <v>0.3228298881107861</v>
+        <v>0.026163848478811858</v>
       </c>
       <c r="D34">
-        <v>-0.015338544958905775</v>
+        <v>0.27675890304734113</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>-0.17145286232246848</v>
+        <v>-0.20326764976519737</v>
       </c>
       <c r="B35">
-        <v>-0.16621219048865424</v>
+        <v>-0.0083878175456799</v>
       </c>
       <c r="C35">
-        <v>0.34000268850039456</v>
+        <v>0.08581626350625123</v>
       </c>
       <c r="D35">
-        <v>0.011531744676281574</v>
+        <v>-0.025238213266202066</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>-0.08320457135635934</v>
+        <v>0.058301254476198515</v>
       </c>
       <c r="B36">
-        <v>-0.08692389793581891</v>
+        <v>0.0004935209170386591</v>
       </c>
       <c r="C36">
-        <v>0.17504172908614934</v>
+        <v>-0.012856955087789161</v>
       </c>
       <c r="D36">
-        <v>0.019308879210410336</v>
+        <v>0.38149985096160466</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>-0.09753433109777317</v>
+        <v>-0.07304874092209913</v>
       </c>
       <c r="B37">
-        <v>-0.13626512992407863</v>
+        <v>-0.0033345372210236927</v>
       </c>
       <c r="C37">
-        <v>0.24673156354351816</v>
+        <v>0.033711025227927</v>
       </c>
       <c r="D37">
-        <v>0.0019326275817267882</v>
+        <v>0.1646884819152452</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>-0.08299935904200262</v>
+        <v>-0.35929326193133426</v>
       </c>
       <c r="B38">
-        <v>-0.08573388250826866</v>
+        <v>-0.008956416539007835</v>
       </c>
       <c r="C38">
-        <v>0.17341982042185763</v>
+        <v>0.11503897450800492</v>
       </c>
       <c r="D38">
-        <v>0.0197713255138142</v>
+        <v>-0.4229159113697763</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>-0.0815157076302305</v>
+        <v>-0.19368209421825822</v>
       </c>
       <c r="B39">
-        <v>-0.09264427885777891</v>
+        <v>-0.007931986255866458</v>
       </c>
       <c r="C39">
-        <v>0.18078559942312297</v>
+        <v>0.08156476432919296</v>
       </c>
       <c r="D39">
-        <v>0.016234810780906248</v>
+        <v>-0.01309343520468719</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>1.0570333351300014</v>
+        <v>-0.1436171443276883</v>
       </c>
       <c r="B40">
-        <v>0.9856761805928369</v>
+        <v>-0.005744685773107539</v>
       </c>
       <c r="C40">
-        <v>-2.0225694608354132</v>
+        <v>0.06031920061762911</v>
       </c>
       <c r="D40">
-        <v>0.12619132521857648</v>
+        <v>0.054574514844519154</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>0.1894867677073241</v>
+        <v>-0.17166561095635569</v>
       </c>
       <c r="B41">
-        <v>0.08670326909236145</v>
+        <v>-0.00513752059157456</v>
       </c>
       <c r="C41">
-        <v>-0.24864803566656907</v>
+        <v>0.061602153569127564</v>
       </c>
       <c r="D41">
-        <v>0.007834997809632184</v>
+        <v>-0.03621159888334295</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>-0.07365872091916616</v>
+        <v>-0.056867424137878576</v>
       </c>
       <c r="B42">
-        <v>-0.0768567076133126</v>
+        <v>-0.002734986416363535</v>
       </c>
       <c r="C42">
-        <v>0.15532883284979665</v>
+        <v>0.02733141568865138</v>
       </c>
       <c r="D42">
-        <v>0.020736506896009387</v>
+        <v>0.1885295779792587</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>0.3488287174757903</v>
+        <v>-0.1709619376860672</v>
       </c>
       <c r="B43">
-        <v>0.3227447255863197</v>
+        <v>-0.00512184852193945</v>
       </c>
       <c r="C43">
-        <v>-0.6615643089113822</v>
+        <v>0.06139087762363328</v>
       </c>
       <c r="D43">
-        <v>0.06142342225692929</v>
+        <v>-0.034825669421478585</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>-0.4143001140028853</v>
+        <v>-0.030547342362179063</v>
       </c>
       <c r="B44">
-        <v>-0.23472479537442922</v>
+        <v>-0.0018059265837023675</v>
       </c>
       <c r="C44">
-        <v>0.5869430296832789</v>
+        <v>0.01718635646497088</v>
       </c>
       <c r="D44">
-        <v>0.00745062902529545</v>
+        <v>0.2283434027041353</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>-0.2578511384333723</v>
+        <v>-0.12624097406290014</v>
       </c>
       <c r="B45">
-        <v>-0.10657688789182275</v>
+        <v>-0.0037298469609493125</v>
       </c>
       <c r="C45">
-        <v>0.3128373249655136</v>
+        <v>0.0453319861407686</v>
       </c>
       <c r="D45">
-        <v>0.022315352135447344</v>
+        <v>0.03901993743761932</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>-0.4734627493731578</v>
+        <v>0.009315705529678931</v>
       </c>
       <c r="B46">
-        <v>-0.37118746617296505</v>
+        <v>-0.0005613938332359517</v>
       </c>
       <c r="C46">
-        <v>0.811761689028236</v>
+        <v>0.0026378155657725143</v>
       </c>
       <c r="D46">
-        <v>-0.009530817701895991</v>
+        <v>0.2922876154980569</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>-0.31647339201166624</v>
+        <v>-0.08595555637430927</v>
       </c>
       <c r="B47">
-        <v>-0.17300699936125513</v>
+        <v>-0.0025743950180798125</v>
       </c>
       <c r="C47">
-        <v>0.4413786373316373</v>
+        <v>0.03140629025559387</v>
       </c>
       <c r="D47">
-        <v>0.01540501187386348</v>
+        <v>0.10813028632355448</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>-0.23757736405872096</v>
+        <v>0.02636342180727586</v>
       </c>
       <c r="B48">
-        <v>-0.08989576762560965</v>
+        <v>-6.399646501471643e-5</v>
       </c>
       <c r="C48">
-        <v>0.27716117632297793</v>
+        <v>-0.0034089824290757026</v>
       </c>
       <c r="D48">
-        <v>0.024138194478039048</v>
+        <v>0.3204146914347122</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>-0.2635720272448177</v>
+        <v>-0.0160189009856339</v>
       </c>
       <c r="B49">
-        <v>-0.11547422557873437</v>
+        <v>-0.0009715811684764703</v>
       </c>
       <c r="C49">
-        <v>0.3287690523604635</v>
+        <v>0.009506869497995623</v>
       </c>
       <c r="D49">
-        <v>0.021465200576094433</v>
+        <v>0.23923880385065613</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>-0.35193954489464885</v>
+        <v>0.038701607015636415</v>
       </c>
       <c r="B50">
-        <v>-0.23184583086633262</v>
+        <v>0.00028944724110880693</v>
       </c>
       <c r="C50">
-        <v>0.5444625423236532</v>
+        <v>-0.007752441434073854</v>
       </c>
       <c r="D50">
-        <v>0.008044677298821615</v>
+        <v>0.3409182046394887</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>-0.313925640333587</v>
+        <v>-0.060724031407228825</v>
       </c>
       <c r="B51">
-        <v>-0.17634259122530604</v>
+        <v>-0.001777220888666512</v>
       </c>
       <c r="C51">
-        <v>0.4444076805046706</v>
+        <v>0.022138776641291845</v>
       </c>
       <c r="D51">
-        <v>0.015005339574966355</v>
+        <v>0.14829642845649038</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
-        <v>-0.24860839216771538</v>
+        <v>-0.013176209226818126</v>
       </c>
       <c r="B52">
-        <v>-0.23291237121440012</v>
+        <v>-0.0006807708100522597</v>
       </c>
       <c r="C52">
-        <v>0.4802437166087869</v>
+        <v>0.007137113331193074</v>
       </c>
       <c r="D52">
-        <v>0.004264323744849843</v>
+        <v>0.23662275736493804</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>-0.18733464990255813</v>
+        <v>-0.05361090739068592</v>
       </c>
       <c r="B53">
-        <v>-0.1805909717042834</v>
+        <v>-0.0015704842282683175</v>
       </c>
       <c r="C53">
-        <v>0.3698137822858243</v>
+        <v>0.019615284939415573</v>
       </c>
       <c r="D53">
-        <v>0.01005947211292924</v>
+        <v>0.16001279064724974</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
-        <v>-0.32001103699563577</v>
+        <v>0.031684375721240735</v>
       </c>
       <c r="B54">
-        <v>-0.200393469542184</v>
+        <v>0.0002314337769529198</v>
       </c>
       <c r="C54">
-        <v>0.4812685977098553</v>
+        <v>-0.006217184224314476</v>
       </c>
       <c r="D54">
-        <v>0.01185454722693509</v>
+        <v>0.32424380599793684</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
-        <v>-0.23333629888821084</v>
+        <v>-0.04244575644567743</v>
       </c>
       <c r="B55">
-        <v>-0.21884340221268772</v>
+        <v>-0.0012173225278074382</v>
       </c>
       <c r="C55">
-        <v>0.45134710958537105</v>
+        <v>0.015451887875320603</v>
       </c>
       <c r="D55">
-        <v>0.005933894910610471</v>
+        <v>0.1772736134426283</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56">
-        <v>-0.12835917802966385</v>
+        <v>-0.3593764369948437</v>
       </c>
       <c r="B56">
-        <v>0.00035787465383403763</v>
+        <v>-0.0071492972040464115</v>
       </c>
       <c r="C56">
-        <v>0.084157354656369</v>
+        <v>0.1031486837246906</v>
       </c>
       <c r="D56">
-        <v>0.03341929490576603</v>
+        <v>-0.4872226928789633</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>-0.2990704175449243</v>
+        <v>-0.35952292359562865</v>
       </c>
       <c r="B57">
-        <v>-0.1732705777149938</v>
+        <v>-0.006506145504601331</v>
       </c>
       <c r="C57">
-        <v>0.43089611474272393</v>
+        <v>0.0989092943346267</v>
       </c>
       <c r="D57">
-        <v>0.015225398389607374</v>
+        <v>-0.5106454331746808</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
-        <v>-0.18676301914353496</v>
+        <v>-0.22921849953298823</v>
       </c>
       <c r="B58">
-        <v>-0.17984825909158103</v>
+        <v>-0.006117291196327813</v>
       </c>
       <c r="C58">
-        <v>0.36844367454698723</v>
+        <v>0.07687504979342424</v>
       </c>
       <c r="D58">
-        <v>0.010169291424169663</v>
+        <v>-0.1604235081646553</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>-0.16603509173286132</v>
+        <v>-0.3353529731745552</v>
       </c>
       <c r="B59">
-        <v>-0.1461285732932155</v>
+        <v>-0.006123971037272239</v>
       </c>
       <c r="C59">
-        <v>0.3093891358488294</v>
+        <v>0.09280052836329923</v>
       </c>
       <c r="D59">
-        <v>0.014969744751939528</v>
+        <v>-0.45650579062224983</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>-0.14775244644718644</v>
+        <v>-0.11706059471726288</v>
       </c>
       <c r="B60">
-        <v>-0.1445636668709035</v>
+        <v>-0.0034255784539939478</v>
       </c>
       <c r="C60">
-        <v>0.29526346407396437</v>
+        <v>0.04191234233662916</v>
       </c>
       <c r="D60">
-        <v>0.013777033255440649</v>
+        <v>0.05351341472789218</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>-0.08561115400216113</v>
+        <v>-0.25830689626031483</v>
       </c>
       <c r="B61">
-        <v>-0.0741386460230874</v>
+        <v>-0.004833633219650687</v>
       </c>
       <c r="C61">
-        <v>0.15993039950643803</v>
+        <v>0.07277278912860823</v>
       </c>
       <c r="D61">
-        <v>0.023112341844984844</v>
+        <v>-0.2871503600041458</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62">
-        <v>-0.0174413872232872</v>
+        <v>-0.06751654356750485</v>
       </c>
       <c r="B62">
-        <v>-0.021961458231076515</v>
+        <v>-0.0019555038394339958</v>
       </c>
       <c r="C62">
-        <v>0.04451397372852767</v>
+        <v>0.024406897202188204</v>
       </c>
       <c r="D62">
-        <v>0.02692271087132238</v>
+        <v>0.13629961750094788</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
-        <v>-0.0693756011448883</v>
+        <v>-0.16396661409234997</v>
       </c>
       <c r="B63">
-        <v>-0.05785342806860749</v>
+        <v>-0.003037286327710666</v>
       </c>
       <c r="C63">
-        <v>0.12736235846294316</v>
+        <v>0.046472823194174576</v>
       </c>
       <c r="D63">
-        <v>0.025017702636905798</v>
+        <v>-0.09038464403490473</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
-        <v>0.590368870640715</v>
+        <v>-0.06527927374200894</v>
       </c>
       <c r="B64">
-        <v>0.5506889285763338</v>
+        <v>-0.0018914741249697613</v>
       </c>
       <c r="C64">
-        <v>-1.1280141031129363</v>
+        <v>0.023626700540299472</v>
       </c>
       <c r="D64">
-        <v>0.08434160837435449</v>
+        <v>0.14007804333277837</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>0.0017205988830533182</v>
+        <v>-0.07283260591127977</v>
       </c>
       <c r="B65">
-        <v>0.009957414177248295</v>
+        <v>-0.0019956134019690945</v>
       </c>
       <c r="C65">
-        <v>-0.01065623270169183</v>
+        <v>0.025491412068948144</v>
       </c>
       <c r="D65">
-        <v>0.032426457004555674</v>
+        <v>0.12308710399007457</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66">
-        <v>0.9215385987488278</v>
+        <v>-0.03847340281340057</v>
       </c>
       <c r="B66">
-        <v>0.8726467413266821</v>
+        <v>-0.0010687056337055681</v>
       </c>
       <c r="C66">
-        <v>-1.7809227020427083</v>
+        <v>0.013808413825844008</v>
       </c>
       <c r="D66">
-        <v>0.11614568869218304</v>
+        <v>0.18250912589401444</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>-0.09904423771054023</v>
+        <v>-0.17172502181176955</v>
       </c>
       <c r="B67">
-        <v>-0.011113259234749057</v>
+        <v>-0.0030882303903441706</v>
       </c>
       <c r="C67">
-        <v>0.08176335152505654</v>
+        <v>0.04799250370893751</v>
       </c>
       <c r="D67">
-        <v>0.03186794423836066</v>
+        <v>-0.11004566988739506</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68">
-        <v>-0.21036970363115629</v>
+        <v>-0.027117292754019983</v>
       </c>
       <c r="B68">
-        <v>-0.11474876492572945</v>
+        <v>-0.0007532581320561064</v>
       </c>
       <c r="C68">
-        <v>0.29460360066753905</v>
+        <v>0.009853522542490356</v>
       </c>
       <c r="D68">
-        <v>0.021089516551633</v>
+        <v>0.20154582360131715</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>-0.0397829587141127</v>
+        <v>-0.1020517212887493</v>
       </c>
       <c r="B69">
-        <v>0.0028163497815251004</v>
+        <v>-0.0019539639483893384</v>
       </c>
       <c r="C69">
-        <v>0.02544988537380033</v>
+        <v>0.029565548865209675</v>
       </c>
       <c r="D69">
-        <v>0.03273228811517109</v>
+        <v>0.039834743403910765</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70">
-        <v>0.04451770096623874</v>
+        <v>-0.010987626347014365</v>
       </c>
       <c r="B70">
-        <v>0.052620439257933756</v>
+        <v>-0.00039367673941539597</v>
       </c>
       <c r="C70">
-        <v>-0.09629066137033515</v>
+        <v>0.004837278066812717</v>
       </c>
       <c r="D70">
-        <v>0.03709320361957405</v>
+        <v>0.23187486654184053</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71">
-        <v>0.04791260765563192</v>
+        <v>-0.16701960536476407</v>
       </c>
       <c r="B71">
-        <v>0.057764495036204386</v>
+        <v>-0.002951428857791456</v>
       </c>
       <c r="C71">
-        <v>-0.10549670540661724</v>
+        <v>0.04632288180615706</v>
       </c>
       <c r="D71">
-        <v>0.03771176988125237</v>
+        <v>-0.10229684246862314</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72">
-        <v>-0.05754794699858085</v>
+        <v>0.0016747453882903092</v>
       </c>
       <c r="B72">
-        <v>-0.04593640644885397</v>
+        <v>-0.00012962070471016256</v>
       </c>
       <c r="C72">
-        <v>0.10356370405197078</v>
+        <v>0.0010232006070926415</v>
       </c>
       <c r="D72">
-        <v>0.026413703854551024</v>
+        <v>0.2563622238555147</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73">
-        <v>-0.10576909569456294</v>
+        <v>-0.16329557290908936</v>
       </c>
       <c r="B73">
-        <v>-0.05022924470605202</v>
+        <v>-0.002709956262439949</v>
       </c>
       <c r="C73">
-        <v>0.14002340270952557</v>
+        <v>0.04395321650015631</v>
       </c>
       <c r="D73">
-        <v>0.027334161615253587</v>
+        <v>-0.10231280710401013</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>0.005150766461496676</v>
+      </c>
+      <c r="B74">
+        <v>-6.021148152484841e-5</v>
+      </c>
+      <c r="C74">
+        <v>-2.907639396888418e-6</v>
+      </c>
+      <c r="D74">
+        <v>0.2631988814948132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>-0.1472465629825932</v>
+      </c>
+      <c r="B75">
+        <v>-0.002268808793048231</v>
+      </c>
+      <c r="C75">
+        <v>0.03828188594044418</v>
+      </c>
+      <c r="D75">
+        <v>-0.07618471190078362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>0.00432724830700999</v>
+      </c>
+      <c r="B76">
+        <v>-6.787840481585693e-5</v>
+      </c>
+      <c r="C76">
+        <v>0.00016969601203974707</v>
+      </c>
+      <c r="D76">
+        <v>0.2611621625289899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>-0.09596172969546732</v>
+      </c>
+      <c r="B77">
+        <v>-0.0012418723867307436</v>
+      </c>
+      <c r="C77">
+        <v>0.02311966317820428</v>
+      </c>
+      <c r="D77">
+        <v>0.0245457327444478</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>-1.8034714989774428e-16</v>
+      </c>
+      <c r="B78">
+        <v>-0.00010427200506372757</v>
+      </c>
+      <c r="C78">
+        <v>0.0010427200506372986</v>
+      </c>
+      <c r="D78">
+        <v>0.25025281215294476</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>-0.08544013205015609</v>
+      </c>
+      <c r="B79">
+        <v>-0.0010697718191086509</v>
+      </c>
+      <c r="C79">
+        <v>0.02030973304672907</v>
+      </c>
+      <c r="D79">
+        <v>0.04696847038116259</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>-0.005368071496885733</v>
+      </c>
+      <c r="B80">
+        <v>-0.00013956985891902852</v>
+      </c>
+      <c r="C80">
+        <v>0.0020398671688165735</v>
+      </c>
+      <c r="D80">
+        <v>0.2361951458629709</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>-0.08536773946210628</v>
+      </c>
+      <c r="B81">
+        <v>-0.0010684723275240398</v>
+      </c>
+      <c r="C81">
+        <v>0.02028935817819832</v>
+      </c>
+      <c r="D81">
+        <v>0.047116307862591814</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>0.014823682430512847</v>
+      </c>
+      <c r="B82">
+        <v>9.616826008052163e-5</v>
+      </c>
+      <c r="C82">
+        <v>-0.002608481194325763</v>
+      </c>
+      <c r="D82">
+        <v>0.28359116812620266</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>-0.005463940176760887</v>
+      </c>
+      <c r="B83">
+        <v>-0.00013862218596597466</v>
+      </c>
+      <c r="C83">
+        <v>0.0020439183624179993</v>
+      </c>
+      <c r="D83">
+        <v>0.23586008429684974</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>-0.04331727155010692</v>
+      </c>
+      <c r="B84">
+        <v>-0.00046987793231500997</v>
+      </c>
+      <c r="C84">
+        <v>0.009742869048382508</v>
+      </c>
+      <c r="D84">
+        <v>0.14069480493732414</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>0.006622863450449006</v>
+      </c>
+      <c r="B85">
+        <v>3.842510398137926e-5</v>
+      </c>
+      <c r="C85">
+        <v>-0.0010518481715878357</v>
+      </c>
+      <c r="D85">
+        <v>0.26231850050505373</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>-0.3647946186146101</v>
+      </c>
+      <c r="B86">
+        <v>-0.005582705789811949</v>
+      </c>
+      <c r="C86">
+        <v>0.09249116394390186</v>
+      </c>
+      <c r="D86">
+        <v>-0.5674872157961732</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>-0.1660645056206637</v>
+      </c>
+      <c r="B87">
+        <v>-0.002777450342712487</v>
+      </c>
+      <c r="C87">
+        <v>0.04485842525319544</v>
+      </c>
+      <c r="D87">
+        <v>-0.10726391945854544</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>-0.13891378993399686</v>
+      </c>
+      <c r="B88">
+        <v>-0.0020005273450575682</v>
+      </c>
+      <c r="C88">
+        <v>0.03500370332991162</v>
+      </c>
+      <c r="D88">
+        <v>-0.064636903904637</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>-0.38031214702693705</v>
+      </c>
+      <c r="B89">
+        <v>-0.004091094129002659</v>
+      </c>
+      <c r="C89">
+        <v>0.08166589556164738</v>
+      </c>
+      <c r="D89">
+        <v>-0.6914147626891619</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>-0.12848958990544906</v>
+      </c>
+      <c r="B90">
+        <v>-0.0017870502451458033</v>
+      </c>
+      <c r="C90">
+        <v>0.03188373709350565</v>
+      </c>
+      <c r="D90">
+        <v>-0.04438760607100047</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>-0.15382317808620807</v>
+      </c>
+      <c r="B91">
+        <v>-0.0019009603591490201</v>
+      </c>
+      <c r="C91">
+        <v>0.03594131406030499</v>
+      </c>
+      <c r="D91">
+        <v>-0.1151113398623351</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>-0.10367576731204212</v>
+      </c>
+      <c r="B92">
+        <v>-0.001361301353387861</v>
+      </c>
+      <c r="C92">
+        <v>0.025118877651017002</v>
+      </c>
+      <c r="D92">
+        <v>0.007729561201727585</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>-0.15317215707783088</v>
+      </c>
+      <c r="B93">
+        <v>-0.0018927702267474808</v>
+      </c>
+      <c r="C93">
+        <v>0.03579122737051982</v>
+      </c>
+      <c r="D93">
+        <v>-0.11357350751708667</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>-0.08184382751720777</v>
+      </c>
+      <c r="B94">
+        <v>-0.000991516271003407</v>
+      </c>
+      <c r="C94">
+        <v>0.019173887755131635</v>
+      </c>
+      <c r="D94">
+        <v>0.05354808197011973</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>-0.11657507721044236</v>
+      </c>
+      <c r="B95">
+        <v>-0.0014371208521530973</v>
+      </c>
+      <c r="C95">
+        <v>0.027343602197450235</v>
+      </c>
+      <c r="D95">
+        <v>-0.027304865786341555</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>-0.38840217501531504</v>
+      </c>
+      <c r="B96">
+        <v>-0.0036651614743222574</v>
+      </c>
+      <c r="C96">
+        <v>0.07833528856766482</v>
+      </c>
+      <c r="D96">
+        <v>-0.7435824567705908</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>-0.15259524583531414</v>
+      </c>
+      <c r="B97">
+        <v>-0.0018846519113252162</v>
+      </c>
+      <c r="C97">
+        <v>0.03564975355379871</v>
+      </c>
+      <c r="D97">
+        <v>-0.11226464199421508</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>-0.10407963052471769</v>
+      </c>
+      <c r="B98">
+        <v>-0.0012701243047084163</v>
+      </c>
+      <c r="C98">
+        <v>0.024344049173578013</v>
+      </c>
+      <c r="D98">
+        <v>0.0014112492274558253</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>-0.23508363292854959</v>
+      </c>
+      <c r="B99">
+        <v>-0.0022861652334101837</v>
+      </c>
+      <c r="C99">
+        <v>0.04840253578303784</v>
+      </c>
+      <c r="D99">
+        <v>-0.3469730276364555</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>-0.08668835563065204</v>
+      </c>
+      <c r="B100">
+        <v>-0.001046652552523773</v>
+      </c>
+      <c r="C100">
+        <v>0.020250085868340036</v>
+      </c>
+      <c r="D100">
+        <v>0.04187843808946082</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>-0.11063910035824123</v>
+      </c>
+      <c r="B101">
+        <v>-0.0011380021751133712</v>
+      </c>
+      <c r="C101">
+        <v>0.02370837864819489</v>
+      </c>
+      <c r="D101">
+        <v>-0.02781783094720791</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>-0.08573190482596177</v>
+      </c>
+      <c r="B102">
+        <v>-0.0010354683734254938</v>
+      </c>
+      <c r="C102">
+        <v>0.02003491693283773</v>
+      </c>
+      <c r="D102">
+        <v>0.04416569528201691</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>-0.1193216611769213</v>
+      </c>
+      <c r="B103">
+        <v>-0.0011513990071933713</v>
+      </c>
+      <c r="C103">
+        <v>0.02476042376200931</v>
+      </c>
+      <c r="D103">
+        <v>-0.05438175103336461</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>-0.06175062984469594</v>
+      </c>
+      <c r="B104">
+        <v>-0.0007149684691888575</v>
+      </c>
+      <c r="C104">
+        <v>0.01421638361871773</v>
+      </c>
+      <c r="D104">
+        <v>0.09876228106113734</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>-0.11475460686602612</v>
+      </c>
+      <c r="B105">
+        <v>-0.0011010631899297139</v>
+      </c>
+      <c r="C105">
+        <v>0.02376437175098966</v>
+      </c>
+      <c r="D105">
+        <v>-0.04325812901860981</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>-0.03678291780626311</v>
+      </c>
+      <c r="B106">
+        <v>-0.0003767492394319559</v>
+      </c>
+      <c r="C106">
+        <v>0.008092370633992164</v>
+      </c>
+      <c r="D106">
+        <v>0.15514127707606676</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>-0.08705761799881521</v>
+      </c>
+      <c r="B107">
+        <v>-0.0008066006444232664</v>
+      </c>
+      <c r="C107">
+        <v>0.017822275617878587</v>
+      </c>
+      <c r="D107">
+        <v>0.024812329873060045</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108">
+        <v>-0.40968972857485864</v>
+      </c>
+      <c r="B108">
+        <v>-0.00291501839871852</v>
+      </c>
+      <c r="C108">
+        <v>0.07200885220986974</v>
+      </c>
+      <c r="D108">
+        <v>-0.8677423711241944</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109">
+        <v>-0.11606706032548982</v>
+      </c>
+      <c r="B109">
+        <v>-0.0011144691520573664</v>
+      </c>
+      <c r="C109">
+        <v>0.02403977948489103</v>
+      </c>
+      <c r="D109">
+        <v>-0.046524485734348926</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>-0.08642957838679188</v>
+      </c>
+      <c r="B110">
+        <v>-0.0007995402268549614</v>
+      </c>
+      <c r="C110">
+        <v>0.017683219182440795</v>
+      </c>
+      <c r="D110">
+        <v>0.02632731109392489</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111">
+        <v>-0.15242443857181</v>
+      </c>
+      <c r="B111">
+        <v>-0.0011957566731867156</v>
+      </c>
+      <c r="C111">
+        <v>0.028402418882582103</v>
+      </c>
+      <c r="D111">
+        <v>-0.15860532886366704</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112">
+        <v>-0.018527636716711655</v>
+      </c>
+      <c r="B112">
+        <v>-0.00016844941959590483</v>
+      </c>
+      <c r="C112">
+        <v>0.003945269651917576</v>
+      </c>
+      <c r="D112">
+        <v>0.19836026251190303</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
+        <v>-0.10186499602575536</v>
+      </c>
+      <c r="B113">
+        <v>-0.0008520748819952442</v>
+      </c>
+      <c r="C113">
+        <v>0.01973833905856704</v>
+      </c>
+      <c r="D113">
+        <v>-0.019914365336783865</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114">
+        <v>-0.4261671663857777</v>
+      </c>
+      <c r="B114">
+        <v>-0.002502346500398265</v>
+      </c>
+      <c r="C114">
+        <v>0.06821661370791013</v>
+      </c>
+      <c r="D114">
+        <v>-0.9579054440669812</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115">
+        <v>-0.22455536043412724</v>
+      </c>
+      <c r="B115">
+        <v>-0.0016607302980393029</v>
+      </c>
+      <c r="C115">
+        <v>0.04043861952906154</v>
+      </c>
+      <c r="D115">
+        <v>-0.35868230053975414</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116">
+        <v>-0.02319321448569504</v>
+      </c>
+      <c r="B116">
+        <v>-0.0001957231132012249</v>
+      </c>
+      <c r="C116">
+        <v>0.004700269850733871</v>
+      </c>
+      <c r="D116">
+        <v>0.18527721671014719</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117">
+        <v>-0.42877688591495566</v>
+      </c>
+      <c r="B117">
+        <v>-0.0024395736391156285</v>
+      </c>
+      <c r="C117">
+        <v>0.06763300552122652</v>
+      </c>
+      <c r="D117">
+        <v>-0.9720940950804255</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118">
+        <v>-0.00382365565213994</v>
+      </c>
+      <c r="B118">
+        <v>-3.323428299799066e-5</v>
+      </c>
+      <c r="C118">
+        <v>0.000896150938748469</v>
+      </c>
+      <c r="D118">
+        <v>0.2349663807957948</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119">
+        <v>-0.038641914942389305</v>
+      </c>
+      <c r="B119">
+        <v>-0.00023438219441126876</v>
+      </c>
+      <c r="C119">
+        <v>0.006498071137415399</v>
+      </c>
+      <c r="D119">
+        <v>0.1371057969467232</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120">
+        <v>-0.4402031906497322</v>
+      </c>
+      <c r="B120">
+        <v>-0.002216903866497498</v>
+      </c>
+      <c r="C120">
+        <v>0.06542087925423516</v>
+      </c>
+      <c r="D120">
+        <v>-1.032371621709991</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121">
+        <v>-0.12188462538372101</v>
+      </c>
+      <c r="B121">
+        <v>-0.0006603593973197545</v>
+      </c>
+      <c r="C121">
+        <v>0.018972086485067905</v>
+      </c>
+      <c r="D121">
+        <v>-0.10345223488047829</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122">
+        <v>-0.030151340309099002</v>
+      </c>
+      <c r="B122">
+        <v>-0.00016378505846917864</v>
+      </c>
+      <c r="C122">
+        <v>0.004839104000225753</v>
+      </c>
+      <c r="D122">
+        <v>0.1589459544689584</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123">
+        <v>-0.12478984506842083</v>
+      </c>
+      <c r="B123">
+        <v>-0.0006681560761762337</v>
+      </c>
+      <c r="C123">
+        <v>0.019306744190647478</v>
+      </c>
+      <c r="D123">
+        <v>-0.11255002502508436</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124">
+        <v>-0.02630169012303941</v>
+      </c>
+      <c r="B124">
+        <v>-0.0001361499253427923</v>
+      </c>
+      <c r="C124">
+        <v>0.004146384089985038</v>
+      </c>
+      <c r="D124">
+        <v>0.16925911173297045</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125">
+        <v>-0.03262221714634993</v>
+      </c>
+      <c r="B125">
+        <v>-0.00016388904003571697</v>
+      </c>
+      <c r="C125">
+        <v>0.005030771165653336</v>
+      </c>
+      <c r="D125">
+        <v>0.1505600896277561</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126">
+        <v>-0.46996323649866084</v>
+      </c>
+      <c r="B126">
+        <v>-0.0017548255374839194</v>
+      </c>
+      <c r="C126">
+        <v>0.060434542171610234</v>
+      </c>
+      <c r="D126">
+        <v>-1.1851961386828636</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127">
+        <v>-0.03798357788052836</v>
+      </c>
+      <c r="B127">
+        <v>-0.00018720938300029514</v>
+      </c>
+      <c r="C127">
+        <v>0.005775567461765906</v>
+      </c>
+      <c r="D127">
+        <v>0.1346579099699992</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128">
+        <v>-0.4790207231772592</v>
+      </c>
+      <c r="B128">
+        <v>-0.0016378376737227946</v>
+      </c>
+      <c r="C128">
+        <v>0.05907245946119253</v>
+      </c>
+      <c r="D128">
+        <v>-1.2308719110225026</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>-0.0353452470129668</v>
+      </c>
+      <c r="B129">
+        <v>-0.0001753907723313483</v>
+      </c>
+      <c r="C129">
+        <v>0.005404172528179095</v>
+      </c>
+      <c r="D129">
+        <v>0.1424493582386798</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130">
+        <v>-0.023560102145362794</v>
+      </c>
+      <c r="B130">
+        <v>-0.00012241191862003448</v>
+      </c>
+      <c r="C130">
+        <v>0.0037338429971773062</v>
+      </c>
+      <c r="D130">
+        <v>0.17716190687954075</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>-0.05613726326802984</v>
+      </c>
+      <c r="B131">
+        <v>-0.000203395881405918</v>
+      </c>
+      <c r="C131">
+        <v>0.007240893378050463</v>
+      </c>
+      <c r="D131">
+        <v>0.0732225173061731</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132">
+        <v>-0.019842693085362007</v>
+      </c>
+      <c r="B132">
+        <v>-0.00010527568909670511</v>
+      </c>
+      <c r="C132">
+        <v>0.0031947425876631156</v>
+      </c>
+      <c r="D132">
+        <v>0.18801764923507755</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133">
+        <v>-0.03209946971217946</v>
+      </c>
+      <c r="B133">
+        <v>-0.00014266430983190417</v>
+      </c>
+      <c r="C133">
+        <v>0.004636590069536946</v>
+      </c>
+      <c r="D133">
+        <v>0.14979752532348345</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>-0.07077969356129196</v>
+      </c>
+      <c r="B134">
+        <v>-0.00023657169482997094</v>
+      </c>
+      <c r="C134">
+        <v>0.008759546538298964</v>
+      </c>
+      <c r="D134">
+        <v>0.0260868247271935</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135">
+        <v>-0.007324354697937752</v>
+      </c>
+      <c r="B135">
+        <v>-4.8408943499528256e-5</v>
+      </c>
+      <c r="C135">
+        <v>0.0013907377948715902</v>
+      </c>
+      <c r="D135">
+        <v>0.22465308174727913</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136">
+        <v>-0.00572089801649305</v>
+      </c>
+      <c r="B136">
+        <v>-4.123504414485187e-5</v>
+      </c>
+      <c r="C136">
+        <v>0.00116116186086147</v>
+      </c>
+      <c r="D136">
+        <v>0.22935600229757527</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137">
+        <v>-0.07163999087012356</v>
+      </c>
+      <c r="B137">
+        <v>-0.00021430766499608376</v>
+      </c>
+      <c r="C137">
+        <v>0.008419229696274984</v>
+      </c>
+      <c r="D137">
+        <v>0.020206151271055826</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138">
+        <v>0.014589959155744608</v>
+      </c>
+      <c r="B138">
+        <v>9.463517372497332e-5</v>
+      </c>
+      <c r="C138">
+        <v>-0.002565098709126651</v>
+      </c>
+      <c r="D138">
+        <v>0.2829789035925189</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139">
+        <v>0.002431283909080344</v>
+      </c>
+      <c r="B139">
+        <v>4.214225442406391e-5</v>
+      </c>
+      <c r="C139">
+        <v>-0.0008451605969660979</v>
+      </c>
+      <c r="D139">
+        <v>0.24718053075653565</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140">
+        <v>-0.5084203983495557</v>
+      </c>
+      <c r="B140">
+        <v>-0.0012757456876594765</v>
+      </c>
+      <c r="C140">
+        <v>0.054500536988768514</v>
+      </c>
+      <c r="D140">
+        <v>-1.3807319368314162</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141">
+        <v>-0.07364592976507633</v>
+      </c>
+      <c r="B141">
+        <v>-0.0002074944846555854</v>
+      </c>
+      <c r="C141">
+        <v>0.008423983831263436</v>
+      </c>
+      <c r="D141">
+        <v>0.012274321627524998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142">
+        <v>-0.07323570852508801</v>
+      </c>
+      <c r="B142">
+        <v>-0.00020386535883757138</v>
+      </c>
+      <c r="C142">
+        <v>0.008333158855669438</v>
+      </c>
+      <c r="D142">
+        <v>0.013244755797106683</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143">
+        <v>-0.0761192633554671</v>
+      </c>
+      <c r="B143">
+        <v>-0.00020932797422752882</v>
+      </c>
+      <c r="C143">
+        <v>0.008610991667087103</v>
+      </c>
+      <c r="D143">
+        <v>0.003805963167753195</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144">
+        <v>0.006137700715619432</v>
+      </c>
+      <c r="B144">
+        <v>6.116536230393338e-5</v>
+      </c>
+      <c r="C144">
+        <v>-0.0014229588900465115</v>
+      </c>
+      <c r="D144">
+        <v>0.2577058269435303</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145">
+        <v>-0.08080749030371205</v>
+      </c>
+      <c r="B145">
+        <v>-0.00021595105167371216</v>
+      </c>
+      <c r="C145">
+        <v>0.009021181029595414</v>
+      </c>
+      <c r="D145">
+        <v>-0.011842477027276335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>